<commit_message>
Added swift cheatshet and some snippits to others
</commit_message>
<xml_diff>
--- a/CSharpCheatSheet.xlsx
+++ b/CSharpCheatSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\CheatSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9E5B5AA-FD27-400F-AF16-75A8D4463A40}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E1284C-726E-425C-B961-18F4E4558D28}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{AB3ACF02-B8F8-4372-8120-4E3760E2D306}"/>
   </bookViews>
@@ -205,12 +205,262 @@
         </r>
       </text>
     </comment>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{05A4BF60-84B8-4C23-BAE9-EBC7CBF436D7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jeremy:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+  &lt;connectionStrings&gt;
+    &lt;add name="</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>GetReal</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>" connectionString="Data Source = localhost; Initial Catalog=</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>getreal</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">; integrated security = true" providerName="System.Data.SqlClient"/&gt;
+  &lt;/connectionStrings&gt;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">OR
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>&lt;connectionStrings&gt;
+        &lt;add name="</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>GetReal</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>" connectionString="server=(local);database=</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>getreal</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>;integrated security= SSPI;" /&gt;
+&lt;/connectionStrings&gt;</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{A5A8BF5F-47D5-41AF-848D-E7E535633B22}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jeremy:
+//Id Example</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+        [Display(Name = </t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>"Id"</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>)]
+        [Required(ErrorMessage = "</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>{0} is required")</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">]
+        [Key]
+        public int ID { get; set; }
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">//Min Value Length Example
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">        [Display(Name = "Category name")]
+        [Required(ErrorMessage = "{0} is required")]
+        [StringLength(int.MaxValue, MinimumLength = 2, ErrorMessage = "{0} length should be longer than {2} characters long.")]
+        public string CategoryName { get; set; }
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">//Mix-Max String Length Example
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">        [Display(Name = "Teaser")]
+        [Required(ErrorMessage = "{0} is required")]
+        [StringLength(150, MinimumLength = 2, ErrorMessage = "{0} length should be between {2} and {1}.")]
+        public string Teaser { get; set; }
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Ntier References</t>
   </si>
@@ -219,6 +469,12 @@
   </si>
   <si>
     <t>Types / ParmStruct Code</t>
+  </si>
+  <si>
+    <t>Webconfig connection string</t>
+  </si>
+  <si>
+    <t>Data Annotations Examples</t>
   </si>
 </sst>
 </file>
@@ -603,15 +859,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1914F946-9DA5-4C77-8D1F-D28FF83408A1}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -629,6 +885,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>